<commit_message>
tested functionality, fixed excel activities
</commit_message>
<xml_diff>
--- a/Invoice_Template.xlsx
+++ b/Invoice_Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28417"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://roboyo-my.sharepoint.com/personal/berna_ural_roboyo_de/Documents/Dokumente/UiPath/BPA_Uebung3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="62" documentId="11_850EE62A66D24965E2BB7950AA0310D26E3D77EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{83EB1E68-3A22-415F-9832-3F1C44BA3A42}"/>
+  <xr:revisionPtr revIDLastSave="117" documentId="11_850EE62A66D24965E2BB7950AA0310D26E3D77EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E1F6464-A08F-42B9-BCD2-C3BCD5C5949F}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Invoice</t>
   </si>
@@ -53,17 +53,20 @@
     <t>Total Amount</t>
   </si>
   <si>
-    <t>Berna Zehra</t>
-  </si>
-  <si>
     <t>€</t>
+  </si>
+  <si>
+    <t>Lance</t>
+  </si>
+  <si>
+    <t>22/12/2024</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -123,7 +126,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -132,7 +135,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="22" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -149,6 +151,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -358,24 +364,24 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" customWidth="1"/>
-    <col min="6" max="6" width="6.42578125" customWidth="1"/>
+    <col min="2" max="2" width="16.81640625" customWidth="1"/>
+    <col min="3" max="3" width="14.54296875" customWidth="1"/>
+    <col min="4" max="4" width="12.81640625" customWidth="1"/>
+    <col min="5" max="5" width="15.54296875" customWidth="1"/>
+    <col min="6" max="6" width="6.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="33.950000000000003" customHeight="1">
+    <row r="1" spans="1:6" ht="34" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -386,25 +392,25 @@
       </c>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="1"/>
       <c r="B2">
-        <v>8974</v>
+        <v>8669</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="8">
-        <v>45646</v>
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
       </c>
       <c r="E2">
         <v>26</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="4"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -412,19 +418,19 @@
       <c r="E3" s="3"/>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
     </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1">
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
@@ -432,5 +438,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
some previous invoices were deleted
</commit_message>
<xml_diff>
--- a/Invoice_Template.xlsx
+++ b/Invoice_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://roboyo-my.sharepoint.com/personal/berna_ural_roboyo_de/Documents/Dokumente/UiPath/BPA_Uebung3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="117" documentId="11_850EE62A66D24965E2BB7950AA0310D26E3D77EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E1F6464-A08F-42B9-BCD2-C3BCD5C5949F}"/>
+  <xr:revisionPtr revIDLastSave="127" documentId="11_850EE62A66D24965E2BB7950AA0310D26E3D77EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{952E2D09-BDD1-4967-A564-EEE520520F09}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,7 +56,7 @@
     <t>€</t>
   </si>
   <si>
-    <t>Lance</t>
+    <t>Levent</t>
   </si>
   <si>
     <t>22/12/2024</t>
@@ -395,7 +395,7 @@
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="1"/>
       <c r="B2">
-        <v>8669</v>
+        <v>3904</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -404,7 +404,7 @@
         <v>7</v>
       </c>
       <c r="E2">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>5</v>

</xml_diff>